<commit_message>
more tests for bsm and mc
</commit_message>
<xml_diff>
--- a/tests/cfi/blackscholes.xlsx
+++ b/tests/cfi/blackscholes.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27920"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miket\PycharmProjects\pyvalfx\tests\cfi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F020A6B0-A1D8-41C7-806A-5B2AF2450549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EF1E1C9-283C-40A8-A4A3-EAF6B543EFCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1AA9BB6B-D9F0-46A3-A13E-8E943A2875C8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{1AA9BB6B-D9F0-46A3-A13E-8E943A2875C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
   <si>
     <t>S</t>
   </si>
@@ -103,7 +104,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.00000000"/>
+    <numFmt numFmtId="164" formatCode="0.00000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -137,7 +138,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,7 +475,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62C01933-6070-48F0-AA98-EA810AE9785A}">
   <dimension ref="A2:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -735,4 +736,756 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FB28520-DE1D-4ACD-B7B8-A1B821557F1F}">
+  <dimension ref="A2:S18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S7" sqref="S7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="12.85546875" customWidth="1"/>
+    <col min="9" max="10" width="12.85546875" customWidth="1"/>
+    <col min="12" max="13" width="12.85546875" customWidth="1"/>
+    <col min="15" max="16" width="12.85546875" customWidth="1"/>
+    <col min="18" max="19" width="12.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>15</v>
+      </c>
+      <c r="F2">
+        <v>10</v>
+      </c>
+      <c r="G2">
+        <v>10</v>
+      </c>
+      <c r="I2">
+        <v>10</v>
+      </c>
+      <c r="J2">
+        <v>10</v>
+      </c>
+      <c r="L2">
+        <v>10</v>
+      </c>
+      <c r="M2">
+        <v>10</v>
+      </c>
+      <c r="O2">
+        <v>10</v>
+      </c>
+      <c r="P2">
+        <v>10</v>
+      </c>
+      <c r="R2">
+        <v>10</v>
+      </c>
+      <c r="S2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>10</v>
+      </c>
+      <c r="G3">
+        <v>15</v>
+      </c>
+      <c r="I3">
+        <v>10</v>
+      </c>
+      <c r="J3">
+        <v>10</v>
+      </c>
+      <c r="L3">
+        <v>10</v>
+      </c>
+      <c r="M3">
+        <v>10</v>
+      </c>
+      <c r="O3">
+        <v>10</v>
+      </c>
+      <c r="P3">
+        <v>10</v>
+      </c>
+      <c r="R3">
+        <v>10</v>
+      </c>
+      <c r="S3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>5</v>
+      </c>
+      <c r="G4">
+        <v>5</v>
+      </c>
+      <c r="I4">
+        <v>5</v>
+      </c>
+      <c r="J4">
+        <v>10</v>
+      </c>
+      <c r="L4">
+        <v>5</v>
+      </c>
+      <c r="M4">
+        <v>5</v>
+      </c>
+      <c r="O4">
+        <v>5</v>
+      </c>
+      <c r="P4">
+        <v>5</v>
+      </c>
+      <c r="R4">
+        <v>5</v>
+      </c>
+      <c r="S4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.45</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.45</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1">
+        <v>0.45</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.45</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0.45</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0.45</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0.45</v>
+      </c>
+      <c r="M5" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="O5" s="1">
+        <v>0.45</v>
+      </c>
+      <c r="P5" s="1">
+        <v>0.45</v>
+      </c>
+      <c r="R5" s="1">
+        <v>0.45</v>
+      </c>
+      <c r="S5" s="1">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="L6" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="M6" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="O6" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="P6" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="R6" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="S6" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0</v>
+      </c>
+      <c r="L7" s="1">
+        <v>0</v>
+      </c>
+      <c r="M7" s="1">
+        <v>0</v>
+      </c>
+      <c r="O7" s="1">
+        <v>0</v>
+      </c>
+      <c r="P7" s="1">
+        <v>0</v>
+      </c>
+      <c r="R7" s="1">
+        <v>0</v>
+      </c>
+      <c r="S7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="2">
+        <f>(LN(C2/C3)+(C6-C7+1/2*C5^2)*C4)/(C5*SQRT(C4))</f>
+        <v>0.75156729243742915</v>
+      </c>
+      <c r="D9" s="2">
+        <f t="shared" ref="D9:F9" si="0">(LN(D2/D3)+(D6-D7+1/2*D5^2)*D4)/(D5*SQRT(D4))</f>
+        <v>1.1545217565414987</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2">
+        <f>(LN(F2/F3)+(F6-F7+1/2*F5^2)*F4)/(F5*SQRT(F4))</f>
+        <v>0.75156729243742915</v>
+      </c>
+      <c r="G9" s="2">
+        <f>(LN(G2/G3)+(G6-G7+1/2*G5^2)*G4)/(G5*SQRT(G4))</f>
+        <v>0.34861282833335955</v>
+      </c>
+      <c r="I9" s="2">
+        <f>(LN(I2/I3)+(I6-I7+1/2*I5^2)*I4)/(I5*SQRT(I4))</f>
+        <v>0.75156729243742915</v>
+      </c>
+      <c r="J9" s="2">
+        <f>(LN(J2/J3)+(J6-J7+1/2*J5^2)*J4)/(J5*SQRT(J4))</f>
+        <v>1.0628766580010385</v>
+      </c>
+      <c r="L9" s="2">
+        <f>(LN(L2/L3)+(L6-L7+1/2*L5^2)*L4)/(L5*SQRT(L4))</f>
+        <v>0.75156729243742915</v>
+      </c>
+      <c r="M9" s="2">
+        <f>(LN(M2/M3)+(M6-M7+1/2*M5^2)*M4)/(M5*SQRT(M4))</f>
+        <v>0.85715939137491926</v>
+      </c>
+      <c r="O9" s="2">
+        <f>(LN(O2/O3)+(O6-O7+1/2*O5^2)*O4)/(O5*SQRT(O4))</f>
+        <v>0.75156729243742915</v>
+      </c>
+      <c r="P9" s="2">
+        <f>(LN(P2/P3)+(P6-P7+1/2*P5^2)*P4)/(P5*SQRT(P4))</f>
+        <v>0.65218649343743851</v>
+      </c>
+      <c r="R9" s="2">
+        <f>(LN(R2/R3)+(R6-R7+1/2*R5^2)*R4)/(R5*SQRT(R4))</f>
+        <v>0.75156729243742915</v>
+      </c>
+      <c r="S9" s="2">
+        <f>(LN(S2/S3)+(S6-S7+1/2*S5^2)*S4)/(S5*SQRT(S4))</f>
+        <v>1.0374680346197409</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="2">
+        <f>C9-(C5*SQRT(C4))</f>
+        <v>-0.2546632974374764</v>
+      </c>
+      <c r="D10" s="2">
+        <f t="shared" ref="D10:F10" si="1">D9-(D5*SQRT(D4))</f>
+        <v>0.14829116666659314</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2">
+        <f>F9-(F5*SQRT(F4))</f>
+        <v>-0.2546632974374764</v>
+      </c>
+      <c r="G10" s="2">
+        <f>G9-(G5*SQRT(G4))</f>
+        <v>-0.65761776154154594</v>
+      </c>
+      <c r="I10" s="2">
+        <f>I9-(I5*SQRT(I4))</f>
+        <v>-0.2546632974374764</v>
+      </c>
+      <c r="J10" s="2">
+        <f>J9-(J5*SQRT(J4))</f>
+        <v>-0.36014828907473229</v>
+      </c>
+      <c r="L10" s="2">
+        <f>L9-(L5*SQRT(L4))</f>
+        <v>-0.2546632974374764</v>
+      </c>
+      <c r="M10" s="2">
+        <f>M9-(M5*SQRT(M4))</f>
+        <v>-0.48448139512495458</v>
+      </c>
+      <c r="O10" s="2">
+        <f>O9-(O5*SQRT(O4))</f>
+        <v>-0.2546632974374764</v>
+      </c>
+      <c r="P10" s="2">
+        <f>P9-(P5*SQRT(P4))</f>
+        <v>-0.35404409643746704</v>
+      </c>
+      <c r="R10" s="2">
+        <f>R9-(R5*SQRT(R4))</f>
+        <v>-0.2546632974374764</v>
+      </c>
+      <c r="S10" s="2">
+        <f>S9-(S5*SQRT(S4))</f>
+        <v>3.1237444744835363E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="2">
+        <f>NORMSDIST(C9)</f>
+        <v>0.77384434056540097</v>
+      </c>
+      <c r="D12" s="2">
+        <f t="shared" ref="D12:F13" si="2">NORMSDIST(D9)</f>
+        <v>0.87585683795048119</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2">
+        <f>NORMSDIST(F9)</f>
+        <v>0.77384434056540097</v>
+      </c>
+      <c r="G12" s="2">
+        <f>NORMSDIST(G9)</f>
+        <v>0.63631000218521128</v>
+      </c>
+      <c r="I12" s="2">
+        <f>NORMSDIST(I9)</f>
+        <v>0.77384434056540097</v>
+      </c>
+      <c r="J12" s="2">
+        <f>NORMSDIST(J9)</f>
+        <v>0.85608105514274724</v>
+      </c>
+      <c r="L12" s="2">
+        <f>NORMSDIST(L9)</f>
+        <v>0.77384434056540097</v>
+      </c>
+      <c r="M12" s="2">
+        <f>NORMSDIST(M9)</f>
+        <v>0.80432159914256762</v>
+      </c>
+      <c r="O12" s="2">
+        <f>NORMSDIST(O9)</f>
+        <v>0.77384434056540097</v>
+      </c>
+      <c r="P12" s="2">
+        <f>NORMSDIST(P9)</f>
+        <v>0.74285956399793496</v>
+      </c>
+      <c r="R12" s="2">
+        <f>NORMSDIST(R9)</f>
+        <v>0.77384434056540097</v>
+      </c>
+      <c r="S12" s="2">
+        <f>NORMSDIST(S9)</f>
+        <v>0.85024110724969082</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="2">
+        <f>NORMSDIST(C10)</f>
+        <v>0.39949158307726518</v>
+      </c>
+      <c r="D13" s="2">
+        <f t="shared" si="2"/>
+        <v>0.55894350686673389</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2">
+        <f>NORMSDIST(F10)</f>
+        <v>0.39949158307726518</v>
+      </c>
+      <c r="G13" s="2">
+        <f>NORMSDIST(G10)</f>
+        <v>0.25539188925987755</v>
+      </c>
+      <c r="I13" s="2">
+        <f>NORMSDIST(I10)</f>
+        <v>0.39949158307726518</v>
+      </c>
+      <c r="J13" s="2">
+        <f>NORMSDIST(J10)</f>
+        <v>0.35936812140447161</v>
+      </c>
+      <c r="L13" s="2">
+        <f>NORMSDIST(L10)</f>
+        <v>0.39949158307726518</v>
+      </c>
+      <c r="M13" s="2">
+        <f>NORMSDIST(M10)</f>
+        <v>0.31402213250250766</v>
+      </c>
+      <c r="O13" s="2">
+        <f>NORMSDIST(O10)</f>
+        <v>0.39949158307726518</v>
+      </c>
+      <c r="P13" s="2">
+        <f>NORMSDIST(P10)</f>
+        <v>0.36165291826582208</v>
+      </c>
+      <c r="R13" s="2">
+        <f>NORMSDIST(R10)</f>
+        <v>0.39949158307726518</v>
+      </c>
+      <c r="S13" s="2">
+        <f>NORMSDIST(S10)</f>
+        <v>0.51245991105638566</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="2">
+        <f>C2*EXP(-C7*C4)*C12-C3*EXP(-C6*C4)*C13</f>
+        <v>4.6271998283439171</v>
+      </c>
+      <c r="D14" s="2">
+        <f t="shared" ref="D14:F14" si="3">D2*EXP(-D7*D4)*D12-D3*EXP(-D6*D4)*D13</f>
+        <v>8.7847961608523235</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2">
+        <f>F2*EXP(-F7*F4)*F12-F3*EXP(-F6*F4)*F13</f>
+        <v>4.6271998283439171</v>
+      </c>
+      <c r="G14" s="2">
+        <f>G2*EXP(-G7*G4)*G12-G3*EXP(-G6*G4)*G13</f>
+        <v>3.3796089716669404</v>
+      </c>
+      <c r="I14" s="2">
+        <f>I2*EXP(-I7*I4)*I12-I3*EXP(-I6*I4)*I13</f>
+        <v>4.6271998283439171</v>
+      </c>
+      <c r="J14" s="2">
+        <f>J2*EXP(-J7*J4)*J12-J3*EXP(-J6*J4)*J13</f>
+        <v>6.3811327138760339</v>
+      </c>
+      <c r="L14" s="2">
+        <f>L2*EXP(-L7*L4)*L12-L3*EXP(-L6*L4)*L13</f>
+        <v>4.6271998283439171</v>
+      </c>
+      <c r="M14" s="2">
+        <f>M2*EXP(-M7*M4)*M12-M3*EXP(-M6*M4)*M13</f>
+        <v>5.5976091644786212</v>
+      </c>
+      <c r="O14" s="2">
+        <f>O2*EXP(-O7*O4)*O12-O3*EXP(-O6*O4)*O13</f>
+        <v>4.6271998283439171</v>
+      </c>
+      <c r="P14" s="2">
+        <f>P2*EXP(-P7*P4)*P12-P3*EXP(-P6*P4)*P13</f>
+        <v>4.3158201254914239</v>
+      </c>
+      <c r="R14" s="2">
+        <f>R2*EXP(-R7*R4)*R12-R3*EXP(-R6*R4)*R13</f>
+        <v>4.6271998283439171</v>
+      </c>
+      <c r="S14" s="2">
+        <f>S2*EXP(-S7*S4)*S12-S3*EXP(-S6*S4)*S13</f>
+        <v>8.8146075557140655</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="2">
+        <f>NORMSDIST(-C9)</f>
+        <v>0.22615565943459898</v>
+      </c>
+      <c r="D16" s="2">
+        <f t="shared" ref="D16:F17" si="4">NORMSDIST(-D9)</f>
+        <v>0.12414316204951885</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2">
+        <f>NORMSDIST(-F9)</f>
+        <v>0.22615565943459898</v>
+      </c>
+      <c r="G16" s="2">
+        <f>NORMSDIST(-G9)</f>
+        <v>0.36368999781478872</v>
+      </c>
+      <c r="I16" s="2">
+        <f>NORMSDIST(-I9)</f>
+        <v>0.22615565943459898</v>
+      </c>
+      <c r="J16" s="2">
+        <f>NORMSDIST(-J9)</f>
+        <v>0.14391894485725273</v>
+      </c>
+      <c r="L16" s="2">
+        <f>NORMSDIST(-L9)</f>
+        <v>0.22615565943459898</v>
+      </c>
+      <c r="M16" s="2">
+        <f>NORMSDIST(-M9)</f>
+        <v>0.19567840085743243</v>
+      </c>
+      <c r="O16" s="2">
+        <f>NORMSDIST(-O9)</f>
+        <v>0.22615565943459898</v>
+      </c>
+      <c r="P16" s="2">
+        <f>NORMSDIST(-P9)</f>
+        <v>0.25714043600206504</v>
+      </c>
+      <c r="R16" s="2">
+        <f>NORMSDIST(-R9)</f>
+        <v>0.22615565943459898</v>
+      </c>
+      <c r="S16" s="2">
+        <f>NORMSDIST(-S9)</f>
+        <v>0.14975889275030918</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="2">
+        <f>NORMSDIST(-C10)</f>
+        <v>0.60050841692273482</v>
+      </c>
+      <c r="D17" s="2">
+        <f t="shared" si="4"/>
+        <v>0.44105649313326611</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2">
+        <f>NORMSDIST(-F10)</f>
+        <v>0.60050841692273482</v>
+      </c>
+      <c r="G17" s="2">
+        <f>NORMSDIST(-G10)</f>
+        <v>0.74460811074012245</v>
+      </c>
+      <c r="I17" s="2">
+        <f>NORMSDIST(-I10)</f>
+        <v>0.60050841692273482</v>
+      </c>
+      <c r="J17" s="2">
+        <f>NORMSDIST(-J10)</f>
+        <v>0.64063187859552839</v>
+      </c>
+      <c r="L17" s="2">
+        <f>NORMSDIST(-L10)</f>
+        <v>0.60050841692273482</v>
+      </c>
+      <c r="M17" s="2">
+        <f>NORMSDIST(-M10)</f>
+        <v>0.68597786749749234</v>
+      </c>
+      <c r="O17" s="2">
+        <f>NORMSDIST(-O10)</f>
+        <v>0.60050841692273482</v>
+      </c>
+      <c r="P17" s="2">
+        <f>NORMSDIST(-P10)</f>
+        <v>0.63834708173417787</v>
+      </c>
+      <c r="R17" s="2">
+        <f>NORMSDIST(-R10)</f>
+        <v>0.60050841692273482</v>
+      </c>
+      <c r="S17" s="2">
+        <f>NORMSDIST(-S10)</f>
+        <v>0.48754008894361434</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="2">
+        <f>C3*EXP(-C6*C4)*C17-C2*EXP(-C7*C4)*C16</f>
+        <v>2.4152076590579661</v>
+      </c>
+      <c r="D18" s="2">
+        <f t="shared" ref="D18:F18" si="5">D3*EXP(-D6*D4)*D17-D2*EXP(-D7*D4)*D16</f>
+        <v>1.572803991566371</v>
+      </c>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2">
+        <f>F3*EXP(-F6*F4)*F17-F2*EXP(-F7*F4)*F16</f>
+        <v>2.4152076590579661</v>
+      </c>
+      <c r="G18" s="2">
+        <f>G3*EXP(-G6*G4)*G17-G2*EXP(-G7*G4)*G16</f>
+        <v>5.0616207177380126</v>
+      </c>
+      <c r="I18" s="2">
+        <f>I3*EXP(-I6*I4)*I17-I2*EXP(-I7*I4)*I16</f>
+        <v>2.4152076590579661</v>
+      </c>
+      <c r="J18" s="2">
+        <f>J3*EXP(-J6*J4)*J17-J2*EXP(-J7*J4)*J16</f>
+        <v>2.4464393110023677</v>
+      </c>
+      <c r="L18" s="2">
+        <f>L3*EXP(-L6*L4)*L17-L2*EXP(-L7*L4)*L16</f>
+        <v>2.4152076590579661</v>
+      </c>
+      <c r="M18" s="2">
+        <f>M3*EXP(-M6*M4)*M17-M2*EXP(-M7*M4)*M16</f>
+        <v>3.3856169951926702</v>
+      </c>
+      <c r="O18" s="2">
+        <f>O3*EXP(-O6*O4)*O17-O2*EXP(-O7*O4)*O16</f>
+        <v>2.4152076590579661</v>
+      </c>
+      <c r="P18" s="2">
+        <f>P3*EXP(-P6*P4)*P17-P2*EXP(-P7*P4)*P16</f>
+        <v>2.9228998897420015</v>
+      </c>
+      <c r="R18" s="2">
+        <f>R3*EXP(-R6*R4)*R17-R2*EXP(-R7*R4)*R16</f>
+        <v>2.4152076590579661</v>
+      </c>
+      <c r="S18" s="2">
+        <f>S3*EXP(-S6*S4)*S17-S2*EXP(-S7*S4)*S16</f>
+        <v>2.1602169525709236</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
round out tests for bs and mc
</commit_message>
<xml_diff>
--- a/tests/cfi/blackscholes.xlsx
+++ b/tests/cfi/blackscholes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27920"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miket\PycharmProjects\pyvalfx\tests\cfi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EF1E1C9-283C-40A8-A4A3-EAF6B543EFCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC61169-52BB-4292-9A9A-069DEC9CFB8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{1AA9BB6B-D9F0-46A3-A13E-8E943A2875C8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1AA9BB6B-D9F0-46A3-A13E-8E943A2875C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -473,19 +473,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62C01933-6070-48F0-AA98-EA810AE9785A}">
-  <dimension ref="A2:E18"/>
+  <dimension ref="A2:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="12.85546875" customWidth="1"/>
+    <col min="3" max="6" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -501,8 +501,11 @@
       <c r="E2">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -518,8 +521,11 @@
       <c r="E3">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -535,8 +541,11 @@
       <c r="E4">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -552,8 +561,11 @@
       <c r="E5" s="1">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="1">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -569,8 +581,11 @@
       <c r="E6" s="1">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="1">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -586,8 +601,11 @@
       <c r="E7" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="1">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -603,8 +621,12 @@
         <f t="shared" si="0"/>
         <v>1.2077913728063143</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="2">
+        <f t="shared" ref="F9" si="1">(LN(F2/F3)+(F6-F7+1/2*F5^2)*F4)/(F5*SQRT(F4))</f>
+        <v>0.60249609393744319</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -613,20 +635,25 @@
         <v>-0.2546632974374764</v>
       </c>
       <c r="D10" s="2">
-        <f t="shared" ref="D10:E10" si="1">D9-(D5*SQRT(D4))</f>
+        <f t="shared" ref="D10:E10" si="2">D9-(D5*SQRT(D4))</f>
         <v>0.43971445909186291</v>
       </c>
       <c r="E10" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-1.3377930394652571</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" s="2">
+        <f t="shared" ref="F10" si="3">F9-(F5*SQRT(F4))</f>
+        <v>-0.40373449593746236</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -635,15 +662,19 @@
         <v>0.77384434056540097</v>
       </c>
       <c r="D12" s="2">
-        <f t="shared" ref="D12:E12" si="2">NORMSDIST(D9)</f>
+        <f t="shared" ref="D12:E12" si="4">NORMSDIST(D9)</f>
         <v>0.78410275921225248</v>
       </c>
       <c r="E12" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.88643623962167872</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" s="2">
+        <f t="shared" ref="F12" si="5">NORMSDIST(F9)</f>
+        <v>0.72657801876382888</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -652,15 +683,19 @@
         <v>0.39949158307726518</v>
       </c>
       <c r="D13" s="2">
-        <f t="shared" ref="D13:E13" si="3">NORMSDIST(D10)</f>
+        <f t="shared" ref="D13:E13" si="6">NORMSDIST(D10)</f>
         <v>0.66992803552159108</v>
       </c>
       <c r="E13" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>9.0481955761883073E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" s="2">
+        <f t="shared" ref="F13" si="7">NORMSDIST(F10)</f>
+        <v>0.34320398494166438</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -669,20 +704,25 @@
         <v>4.6271998283439171</v>
       </c>
       <c r="D14" s="2">
-        <f t="shared" ref="D14:E14" si="4">D2*EXP(-D7*D4)*D12-D3*EXP(-D6*D4)*D13</f>
+        <f t="shared" ref="D14:E14" si="8">D2*EXP(-D7*D4)*D12-D3*EXP(-D6*D4)*D13</f>
         <v>7.2698660295962121</v>
       </c>
       <c r="E14" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>7.7967279863254584</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" s="2">
+        <f t="shared" ref="F14" si="9">F2*EXP(-F7*F4)*F12-F3*EXP(-F6*F4)*F13</f>
+        <v>3.9574398326343001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -691,15 +731,19 @@
         <v>0.22615565943459898</v>
       </c>
       <c r="D16" s="2">
-        <f t="shared" ref="D16:E16" si="5">NORMSDIST(-D9)</f>
+        <f t="shared" ref="D16:E16" si="10">NORMSDIST(-D9)</f>
         <v>0.21589724078774758</v>
       </c>
       <c r="E16" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.11356376037832125</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" s="2">
+        <f t="shared" ref="F16" si="11">NORMSDIST(-F9)</f>
+        <v>0.27342198123617106</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -708,15 +752,19 @@
         <v>0.60050841692273482</v>
       </c>
       <c r="D17" s="2">
-        <f t="shared" ref="D17:E17" si="6">NORMSDIST(-D10)</f>
+        <f t="shared" ref="D17:E17" si="12">NORMSDIST(-D10)</f>
         <v>0.33007196447840892</v>
       </c>
       <c r="E17" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.90951804423811689</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" s="2">
+        <f t="shared" ref="F17" si="13">NORMSDIST(-F10)</f>
+        <v>0.65679601505833562</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -725,12 +773,16 @@
         <v>2.4152076590579661</v>
       </c>
       <c r="D18" s="2">
-        <f t="shared" ref="D18:E18" si="7">D3*EXP(-D6*D4)*D17-D2*EXP(-D7*D4)*D16</f>
+        <f t="shared" ref="D18:E18" si="14">D3*EXP(-D6*D4)*D17-D2*EXP(-D7*D4)*D16</f>
         <v>1.5310043683089178</v>
       </c>
       <c r="E18" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="14"/>
         <v>9.5961459023237587</v>
+      </c>
+      <c r="F18" s="2">
+        <f t="shared" ref="F18" si="15">F3*EXP(-F6*F4)*F17-F2*EXP(-F7*F4)*F16</f>
+        <v>3.052225351877738</v>
       </c>
     </row>
   </sheetData>
@@ -742,7 +794,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FB28520-DE1D-4ACD-B7B8-A1B821557F1F}">
   <dimension ref="A2:S18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
@@ -1032,7 +1084,7 @@
         <v>0.75156729243742915</v>
       </c>
       <c r="D9" s="2">
-        <f t="shared" ref="D9:F9" si="0">(LN(D2/D3)+(D6-D7+1/2*D5^2)*D4)/(D5*SQRT(D4))</f>
+        <f t="shared" ref="D9" si="0">(LN(D2/D3)+(D6-D7+1/2*D5^2)*D4)/(D5*SQRT(D4))</f>
         <v>1.1545217565414987</v>
       </c>
       <c r="E9" s="2"/>
@@ -1086,7 +1138,7 @@
         <v>-0.2546632974374764</v>
       </c>
       <c r="D10" s="2">
-        <f t="shared" ref="D10:F10" si="1">D9-(D5*SQRT(D4))</f>
+        <f t="shared" ref="D10" si="1">D9-(D5*SQRT(D4))</f>
         <v>0.14829116666659314</v>
       </c>
       <c r="E10" s="2"/>
@@ -1155,7 +1207,7 @@
         <v>0.77384434056540097</v>
       </c>
       <c r="D12" s="2">
-        <f t="shared" ref="D12:F13" si="2">NORMSDIST(D9)</f>
+        <f t="shared" ref="D12:D13" si="2">NORMSDIST(D9)</f>
         <v>0.87585683795048119</v>
       </c>
       <c r="E12" s="2"/>
@@ -1263,7 +1315,7 @@
         <v>4.6271998283439171</v>
       </c>
       <c r="D14" s="2">
-        <f t="shared" ref="D14:F14" si="3">D2*EXP(-D7*D4)*D12-D3*EXP(-D6*D4)*D13</f>
+        <f t="shared" ref="D14" si="3">D2*EXP(-D7*D4)*D12-D3*EXP(-D6*D4)*D13</f>
         <v>8.7847961608523235</v>
       </c>
       <c r="E14" s="2"/>
@@ -1332,7 +1384,7 @@
         <v>0.22615565943459898</v>
       </c>
       <c r="D16" s="2">
-        <f t="shared" ref="D16:F17" si="4">NORMSDIST(-D9)</f>
+        <f t="shared" ref="D16:D17" si="4">NORMSDIST(-D9)</f>
         <v>0.12414316204951885</v>
       </c>
       <c r="E16" s="2"/>
@@ -1440,7 +1492,7 @@
         <v>2.4152076590579661</v>
       </c>
       <c r="D18" s="2">
-        <f t="shared" ref="D18:F18" si="5">D3*EXP(-D6*D4)*D17-D2*EXP(-D7*D4)*D16</f>
+        <f t="shared" ref="D18" si="5">D3*EXP(-D6*D4)*D17-D2*EXP(-D7*D4)*D16</f>
         <v>1.572803991566371</v>
       </c>
       <c r="E18" s="2"/>

</xml_diff>